<commit_message>
Canvis Filtre subdep, etc
Creació de filtre de subdepartament
</commit_message>
<xml_diff>
--- a/tmi/bd-telefonia/arxiu_telefonia.xlsx
+++ b/tmi/bd-telefonia/arxiu_telefonia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecnicasmecanicas-my.sharepoint.com/personal/itpractice_tmipal_com/Documents/Documentos/GitHub/portafoli/Web extensions telefòniques/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tecnicasmecanicas-my.sharepoint.com/personal/itpractice_tmipal_com/Documents/Documentos/GitHub/portafoli/tmi/bd-telefonia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{A60219CD-EBD2-437F-A6AE-BCA018802907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C70307-F015-43FC-A6A9-DEFF26379724}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{A60219CD-EBD2-437F-A6AE-BCA018802907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08CD1357-A946-4E04-BFB8-AEF40E2E61F8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4B81C1B4-1ED8-4653-9717-BF60D5D93CDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4B81C1B4-1ED8-4653-9717-BF60D5D93CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="ListadoPuestos-CGIPIPCENTREX001" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="755">
   <si>
     <t>Webex</t>
   </si>
@@ -2289,6 +2289,33 @@
   </si>
   <si>
     <t>Riera</t>
+  </si>
+  <si>
+    <t>Automatismes</t>
+  </si>
+  <si>
+    <t>Comercial</t>
+  </si>
+  <si>
+    <t>Administracio</t>
+  </si>
+  <si>
+    <t>Logistica</t>
+  </si>
+  <si>
+    <t>Compres</t>
+  </si>
+  <si>
+    <t>Taller, MachineAssembly</t>
+  </si>
+  <si>
+    <t>Enginyeria</t>
+  </si>
+  <si>
+    <t>Taller, LineAssembly</t>
+  </si>
+  <si>
+    <t>Enginyeria, PMO</t>
   </si>
 </sst>
 </file>
@@ -2900,8 +2927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B924CCF6-ACEC-41F7-BE2D-2D2C72A9ACED}">
   <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K108" sqref="K108"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,7 +3023,7 @@
         <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>746</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
@@ -3038,7 +3065,7 @@
         <v>24</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>746</v>
       </c>
       <c r="M3" t="s">
         <v>14</v>
@@ -3080,7 +3107,7 @@
         <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>746</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
@@ -3122,7 +3149,7 @@
         <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="M5" t="s">
         <v>14</v>
@@ -3164,7 +3191,7 @@
         <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>37</v>
+        <v>747</v>
       </c>
       <c r="M6" t="s">
         <v>14</v>
@@ -3206,7 +3233,7 @@
         <v>41</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>748</v>
       </c>
       <c r="M7" t="s">
         <v>14</v>
@@ -3248,7 +3275,7 @@
         <v>46</v>
       </c>
       <c r="L8" t="s">
-        <v>47</v>
+        <v>749</v>
       </c>
       <c r="M8" t="s">
         <v>14</v>
@@ -3290,7 +3317,7 @@
         <v>50</v>
       </c>
       <c r="L9" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="M9" t="s">
         <v>14</v>
@@ -3332,7 +3359,7 @@
         <v>55</v>
       </c>
       <c r="L10" t="s">
-        <v>56</v>
+        <v>747</v>
       </c>
       <c r="M10" t="s">
         <v>14</v>
@@ -3416,7 +3443,7 @@
         <v>64</v>
       </c>
       <c r="L12" t="s">
-        <v>56</v>
+        <v>747</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -3458,7 +3485,7 @@
         <v>68</v>
       </c>
       <c r="L13" t="s">
-        <v>56</v>
+        <v>750</v>
       </c>
       <c r="M13" t="s">
         <v>14</v>
@@ -3500,7 +3527,7 @@
         <v>72</v>
       </c>
       <c r="L14" t="s">
-        <v>56</v>
+        <v>751</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
@@ -3542,7 +3569,7 @@
         <v>76</v>
       </c>
       <c r="L15" t="s">
-        <v>56</v>
+        <v>747</v>
       </c>
       <c r="M15" t="s">
         <v>14</v>
@@ -3668,7 +3695,7 @@
         <v>88</v>
       </c>
       <c r="L18" t="s">
-        <v>56</v>
+        <v>752</v>
       </c>
       <c r="M18" t="s">
         <v>14</v>
@@ -3752,7 +3779,7 @@
         <v>96</v>
       </c>
       <c r="L20" t="s">
-        <v>56</v>
+        <v>753</v>
       </c>
       <c r="M20" t="s">
         <v>14</v>
@@ -3794,7 +3821,7 @@
         <v>100</v>
       </c>
       <c r="L21" t="s">
-        <v>56</v>
+        <v>754</v>
       </c>
       <c r="M21" t="s">
         <v>14</v>
@@ -3836,7 +3863,7 @@
         <v>103</v>
       </c>
       <c r="L22" t="s">
-        <v>56</v>
+        <v>754</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>

</xml_diff>